<commit_message>
Uploading Cleansed datasets from .cvs worksheets. Stopped at splitting columns with Flash Fill
</commit_message>
<xml_diff>
--- a/CSV_ETL_Training/LL_Files_Excel_Managing_and_Analyzing_Data/LL_Files_Excel_Managing_and_Analyzing_Data/Exercise Files/1Checking_Data_Quality/01_04/Find duplicates using formulas.xlsx
+++ b/CSV_ETL_Training/LL_Files_Excel_Managing_and_Analyzing_Data/LL_Files_Excel_Managing_and_Analyzing_Data/Exercise Files/1Checking_Data_Quality/01_04/Find duplicates using formulas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/emgarcia/Downloads/01_04/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmon\terminal_prework\git\codingdemo\CSV_ETL_Training\LL_Files_Excel_Managing_and_Analyzing_Data\LL_Files_Excel_Managing_and_Analyzing_Data\Exercise Files\1Checking_Data_Quality\01_04\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7042D289-A870-6141-ACF5-1A3D4538EB39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F77956E-7897-49DE-87B2-FAACDDCE441B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4300" yWindow="1360" windowWidth="22140" windowHeight="12540" xr2:uid="{543F5EBD-DE74-4358-97D5-CA9BFBDEDE7E}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{543F5EBD-DE74-4358-97D5-CA9BFBDEDE7E}"/>
   </bookViews>
   <sheets>
     <sheet name="Cities" sheetId="1" r:id="rId1"/>
@@ -36,8 +36,28 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>tc={C9AF3638-9517-49A2-9951-00D94F862262}</author>
+  </authors>
+  <commentList>
+    <comment ref="H1" authorId="0" shapeId="0" xr:uid="{C9AF3638-9517-49A2-9951-00D94F862262}">
+      <text>
+        <t>[Threaded comment]
+Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
+Comment:
+    Used =IF(AND( Formula to tag duplicate data that was incomplete and then removed the duplicate values from the dataset.
+Data set still has poor data quality due to multiple entries missing critical value of distance.
+Would not recommend performing an analysis on this incomplete dataset. Outside of Identifying areas of missing data.</t>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="51">
   <si>
     <t>City</t>
   </si>
@@ -178,13 +198,25 @@
   </si>
   <si>
     <t>LOS</t>
+  </si>
+  <si>
+    <t>Original Dataset</t>
+  </si>
+  <si>
+    <t>Cleansed Data</t>
+  </si>
+  <si>
+    <t>Cleansed Dataset</t>
+  </si>
+  <si>
+    <t>Checks</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="16"/>
       <color theme="1"/>
@@ -206,6 +238,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -215,7 +253,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -223,13 +261,52 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -245,6 +322,12 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <person displayName="Edwin Edmondson" id="{25D7B93A-B2D5-483F-91AD-8F8B3F6AC9EC}" userId="2246e878118cfc47" providerId="Windows Live"/>
+</personList>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -521,163 +604,238 @@
 </a:theme>
 </file>
 
+<file path=xl/threadedComments/threadedComment1.xml><?xml version="1.0" encoding="utf-8"?>
+<ThreadedComments xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <threadedComment ref="H1" dT="2023-02-01T17:17:41.33" personId="{25D7B93A-B2D5-483F-91AD-8F8B3F6AC9EC}" id="{C9AF3638-9517-49A2-9951-00D94F862262}">
+    <text>Used =IF(AND( Formula to tag duplicate data that was incomplete and then removed the duplicate values from the dataset.
+Data set still has poor data quality due to multiple entries missing critical value of distance.
+Would not recommend performing an analysis on this incomplete dataset. Outside of Identifying areas of missing data.</text>
+  </threadedComment>
+</ThreadedComments>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42786D73-B668-461E-B123-FAF1C2BC1944}">
-  <dimension ref="C1:C28"/>
+  <dimension ref="C1:E29"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.5" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="3" max="3" width="16.5546875" customWidth="1"/>
     <col min="5" max="5" width="24.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C1" s="1" t="s">
+    <row r="1" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C1" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+      <c r="E2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C3" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="E4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="7" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:5" x14ac:dyDescent="0.4">
       <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C10" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C10" t="s">
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C11" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="11" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C11" t="s">
+      <c r="E11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C12" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C12" t="s">
+      <c r="E12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C13" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C13" t="s">
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C14" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="14" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C14" t="s">
+      <c r="E14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C15" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="15" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C15" t="s">
+      <c r="E15" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C16" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C16" t="s">
+      <c r="E16" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C17" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C17" t="s">
+      <c r="E17" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C18" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="18" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C18" t="s">
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C19" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="19" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C19" t="s">
+      <c r="E19" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C20" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C20" t="s">
+      <c r="E20" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C21" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C21" t="s">
+    <row r="22" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" t="s">
+    <row r="23" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C23" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C23" t="s">
+    <row r="24" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C24" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C24" t="s">
+    <row r="25" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C25" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C25" t="s">
+    <row r="26" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C26" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C26" t="s">
+    <row r="27" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C27" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C27" t="s">
+    <row r="28" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C28" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C28" t="s">
+    <row r="29" spans="3:5" x14ac:dyDescent="0.4">
+      <c r="C29" t="s">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E2:E13">
-    <sortCondition ref="E3:E13"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="E3:E14">
+    <sortCondition ref="E4:E14"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -685,279 +843,647 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC8A63-0D32-4229-89B4-879C80485077}">
-  <dimension ref="B1:D32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AADC8A63-0D32-4229-89B4-879C80485077}">
+  <dimension ref="B1:J34"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="20.5" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="15.21875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B1" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="H1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
+    </row>
+    <row r="2" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+    </row>
+    <row r="3" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="5" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+      <c r="E3" s="4"/>
+      <c r="F3" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C4" s="6" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6" t="str">
+        <f>IF(AND(B4=B5,C4=C5),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B5" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C5" s="6" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6" t="str">
+        <f>IF(AND(B5=B6,C5=C6),"Look","")</f>
+        <v>Look</v>
+      </c>
+      <c r="H5" t="s">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="I5" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="J5" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6" t="str">
+        <f>IF(AND(B6=B7,C6=C7),"Look","")</f>
+        <v>Look</v>
+      </c>
+      <c r="H6" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B7" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="E7" s="6"/>
+      <c r="F7" s="6" t="str">
+        <f>IF(AND(B7=B8,C7=C8),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H7" t="s">
+        <v>2</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B8" s="6" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6" t="str">
+        <f>IF(AND(B8=B9,C8=C9),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B9" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C9" s="6" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6" t="str">
+        <f>IF(AND(B9=B10,C9=C10),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H9" t="s">
         <v>10</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B10" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6" t="str">
+        <f>IF(AND(B10=B11,C10=C11),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H10" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B11" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6" t="str">
+        <f>IF(AND(B11=B12,C11=C12),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H11" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B12" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C12" s="6" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6" t="str">
+        <f>IF(AND(B12=B13,C12=C13),"Look","")</f>
+        <v>Look</v>
+      </c>
+      <c r="H12" t="s">
+        <v>13</v>
+      </c>
+      <c r="I12" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B13" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C13" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="D11" t="s">
+      <c r="D13" s="6" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="E13" s="6"/>
+      <c r="F13" s="6" t="str">
+        <f>IF(AND(B13=B14,C13=C14),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H13" t="s">
+        <v>1</v>
+      </c>
+      <c r="I13" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B14" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C14" s="6" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6" t="str">
+        <f>IF(AND(B14=B15,C14=C15),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H14" t="s">
+        <v>12</v>
+      </c>
+      <c r="I14" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C15" s="6" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6" t="str">
+        <f>IF(AND(B15=B16,C15=C16),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H15" t="s">
+        <v>9</v>
+      </c>
+      <c r="I15" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B16" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C16" s="6" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6" t="str">
+        <f>IF(AND(B16=B17,C16=C17),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H16" t="s">
+        <v>16</v>
+      </c>
+      <c r="I16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B17" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C17" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6" t="str">
+        <f>IF(AND(B17=B18,C17=C18),"Look","")</f>
+        <v>Look</v>
+      </c>
+      <c r="H17" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B18" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C18" s="6" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6" t="str">
+        <f>IF(AND(B18=B19,C18=C19),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B19" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C19" s="6" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6" t="str">
+        <f>IF(AND(B19=B20,C19=C20),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H19" t="s">
+        <v>15</v>
+      </c>
+      <c r="I19" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B20" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C20" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6" t="str">
+        <f>IF(AND(B20=B21,C20=C21),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H20" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="21" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B21" s="6" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="C21" s="6"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="6"/>
+      <c r="F21" s="6" t="str">
+        <f>IF(AND(B21=B22,C21=C22),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H21" t="s">
+        <v>11</v>
+      </c>
+      <c r="I21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J21" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="22" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6" t="str">
+        <f>IF(AND(B22=B23,C22=C23),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H22" t="s">
+        <v>8</v>
+      </c>
+      <c r="I22" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="23" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B23" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C23" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="D21" t="s">
+      <c r="D23" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+      <c r="E23" s="6"/>
+      <c r="F23" s="6" t="str">
+        <f>IF(AND(B23=B24,C23=C24),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H23" t="s">
+        <v>5</v>
+      </c>
+      <c r="I23" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B24" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6" t="str">
+        <f>IF(AND(B24=B25,C24=C25),"Look","")</f>
+        <v>Look</v>
+      </c>
+      <c r="H24" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B25" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+      <c r="C25" s="6"/>
+      <c r="D25" s="6"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6" t="str">
+        <f>IF(AND(B25=B26,C25=C26),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H25" t="s">
+        <v>19</v>
+      </c>
+      <c r="I25" t="s">
+        <v>37</v>
+      </c>
+      <c r="J25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B26" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C26" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6" t="str">
+        <f>IF(AND(B26=B27,C26=C27),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H26" t="s">
+        <v>41</v>
+      </c>
+      <c r="I26" t="s">
+        <v>42</v>
+      </c>
+      <c r="J26" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B27" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C27" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="D25" t="s">
+      <c r="D27" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+      <c r="E27" s="6"/>
+      <c r="F27" s="6" t="str">
+        <f>IF(AND(B27=B28,C27=C28),"Look","")</f>
+        <v/>
+      </c>
+      <c r="H27" t="s">
+        <v>41</v>
+      </c>
+      <c r="I27" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="28" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B28" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C28" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D26" t="s">
+      <c r="D28" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+      <c r="E28" s="6"/>
+      <c r="F28" s="6" t="str">
+        <f>IF(AND(B28=B29,C28=C29),"Look","")</f>
+        <v>Look</v>
+      </c>
+    </row>
+    <row r="29" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C29" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="D27" t="s">
+      <c r="D29" s="6" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+      <c r="E29" s="6"/>
+      <c r="F29" s="6" t="str">
+        <f>IF(AND(B29=B30,C29=C30),"Look","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="30" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B30" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+      <c r="C30" s="6"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6" t="str">
+        <f>IF(AND(B30=B31,C30=C31),"Look","")</f>
+        <v>Look</v>
+      </c>
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B31" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+      <c r="C31" s="6"/>
+      <c r="D31" s="6"/>
+      <c r="E31" s="6"/>
+      <c r="F31" s="6"/>
+      <c r="G31" t="str">
+        <f t="shared" ref="G5:G34" si="0">IF(AND(B31=B32,C31=C32),"Look","")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.4">
+      <c r="B32" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C32" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B33" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C33" s="6" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+      <c r="F33" s="6"/>
+      <c r="G33" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.4">
+      <c r="B34" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C34" s="7" t="s">
         <v>43</v>
       </c>
+      <c r="D34" s="7"/>
+      <c r="E34" s="7"/>
+      <c r="F34" s="7"/>
+      <c r="G34" t="str">
+        <f t="shared" si="0"/>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:B30">
-    <sortCondition ref="B4:B30"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B4:B32">
+    <sortCondition ref="B6:B32"/>
   </sortState>
+  <mergeCells count="2">
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="H1:J1"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>